<commit_message>
added first iem work folder
</commit_message>
<xml_diff>
--- a/iem/entregas/pratica-ceramicas-1/pratica-ceramicas-1.xlsx
+++ b/iem/entregas/pratica-ceramicas-1/pratica-ceramicas-1.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\juan-cassius\docs\eng-mat-repo\iem\entregas\pratica-ceramicas-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C93F40-BEDF-4968-A40A-990E6B622F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5859AEF6-D2EF-41BF-B4A1-E3D05680113F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Prática cerâmicas 1</t>
   </si>
@@ -132,14 +141,59 @@
     <t>C33</t>
   </si>
   <si>
-    <t>Peso (g)</t>
+    <t>A partir deste corpo de prova não se sabe qual a temperatura de queima dos mesmos</t>
+  </si>
+  <si>
+    <t>Peso seco (g)</t>
+  </si>
+  <si>
+    <t>Peso úmido (g)</t>
+  </si>
+  <si>
+    <t>Peso imerso (g)</t>
+  </si>
+  <si>
+    <t>Porosidade Aparente</t>
+  </si>
+  <si>
+    <t>PA% = ((Pu-Pq)/Pu-Pi))*100</t>
+  </si>
+  <si>
+    <t>Densidade Aparente (g/cm³)</t>
+  </si>
+  <si>
+    <t>DA = (Pq/(Pu-Pi))*ρ água</t>
+  </si>
+  <si>
+    <t>Absorção de água</t>
+  </si>
+  <si>
+    <t>AA% = ((Pu-Pq)/Pq)*100</t>
+  </si>
+  <si>
+    <t>Porosidade Aparente (%)</t>
+  </si>
+  <si>
+    <t>Absorção de Água (%)</t>
+  </si>
+  <si>
+    <t>Módulo de Ruptura</t>
+  </si>
+  <si>
+    <t>Temperatura da água (°C)</t>
+  </si>
+  <si>
+    <t>Densidade da água - ρ (g/mL)</t>
+  </si>
+  <si>
+    <t>*Note, a densidade é relativa a temperatura que a água apresentava no momento do experimento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +203,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,11 +236,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,312 +524,1012 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>8.8800000000000008</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>11.1</v>
+      </c>
+      <c r="D4">
+        <v>5.63</v>
+      </c>
+      <c r="E4" s="4">
+        <f>((C4-B4)/(C4-D4))*100</f>
+        <v>40.585009140767809</v>
+      </c>
+      <c r="F4" s="4">
+        <f>(B4/(C4-D4))*K$8</f>
+        <v>1.6198288848263256</v>
+      </c>
+      <c r="G4" s="4">
+        <f>((C4-B4)/B4)*100</f>
+        <v>24.999999999999986</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>8.77</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>10.97</v>
+      </c>
+      <c r="D5">
+        <v>5.52</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" ref="E5:E36" si="0">((C5-B5)/(C5-D5))*100</f>
+        <v>40.36697247706423</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" ref="F5:F36" si="1">(B5/(C5-D5))*K$8</f>
+        <v>1.6056341284403666</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" ref="G5:G36" si="2">((C5-B5)/B5)*100</f>
+        <v>25.085518814139125</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>8.93</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>11.19</v>
+      </c>
+      <c r="D6">
+        <v>5.65</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>40.794223826714806</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6083671480144408</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="2"/>
+        <v>25.307950727883537</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>8.74</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>10.96</v>
+      </c>
+      <c r="D7">
+        <v>5.52</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>40.808823529411768</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6030830882352938</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="2"/>
+        <v>25.400457665903897</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="J7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>8.94</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>11.22</v>
+      </c>
+      <c r="D8">
+        <v>5.65</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>40.933572710951545</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="1"/>
+        <v>1.601495870736086</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="2"/>
+        <v>25.503355704697999</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="J8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8">
+        <v>0.99780000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <v>8.8699999999999992</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>11.05</v>
+      </c>
+      <c r="D9">
+        <v>5.63</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>40.221402214022163</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6329309963099627</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="2"/>
+        <v>24.577226606538911</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="J9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>8.73</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>10.91</v>
+      </c>
+      <c r="D10">
+        <v>5.54</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>40.595903165735564</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6221217877094973</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="2"/>
+        <v>24.971363115693006</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
         <v>8.9700000000000006</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>11.21</v>
+      </c>
+      <c r="D11">
+        <v>5.68</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>40.506329113924046</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6184929475587702</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="2"/>
+        <v>24.972129319955407</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
         <v>8.81</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>11.06</v>
+      </c>
+      <c r="D12">
+        <v>5.58</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>41.058394160583937</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6041273722627736</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="2"/>
+        <v>25.539160045402948</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
         <v>8.83</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>11.05</v>
+      </c>
+      <c r="D13">
+        <v>5.62</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>40.883977900552495</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6225734806629832</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="2"/>
+        <v>25.141562853907139</v>
+      </c>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
         <v>8.81</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>10.72</v>
+      </c>
+      <c r="D14">
+        <v>5.6</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>37.304687499999993</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="1"/>
+        <v>1.7169175781249999</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="2"/>
+        <v>21.679909194097615</v>
+      </c>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
         <v>8.92</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>10.94</v>
+      </c>
+      <c r="D15">
+        <v>5.69</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>38.476190476190474</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6953097142857145</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="2"/>
+        <v>22.645739910313896</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16">
         <v>8.83</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>10.86</v>
+      </c>
+      <c r="D16">
+        <v>5.59</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>38.519924098671716</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6718356736242888</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="2"/>
+        <v>22.989807474518678</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
         <v>8.84</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>10.95</v>
+      </c>
+      <c r="D17">
+        <v>5.67</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>39.962121212121204</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="1"/>
+        <v>1.670559090909091</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="2"/>
+        <v>23.86877828054298</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
         <v>8.1199999999999992</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>10.07</v>
+      </c>
+      <c r="D18">
+        <v>5.2</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
+        <v>40.041067761807</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="1"/>
+        <v>1.66368295687885</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="2"/>
+        <v>24.014778325123167</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
         <v>8.08</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="D19">
+        <v>5.12</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="0"/>
+        <v>36.616702355460376</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="1"/>
+        <v>1.7263862955032123</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="2"/>
+        <v>21.163366336633651</v>
+      </c>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20">
         <v>8.07</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>9.81</v>
+      </c>
+      <c r="D20">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
+        <v>37.021276595744688</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="1"/>
+        <v>1.7132438297872341</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="2"/>
+        <v>21.561338289962826</v>
+      </c>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21">
         <v>8.1300000000000008</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="D21">
+        <v>5.14</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="0"/>
+        <v>37.83783783783781</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6865101871101873</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="2"/>
+        <v>22.386223862238602</v>
+      </c>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22">
         <v>8.14</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>9.98</v>
+      </c>
+      <c r="D22">
+        <v>5.51</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="0"/>
+        <v>41.163310961968669</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8170228187919464</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="2"/>
+        <v>22.604422604422599</v>
+      </c>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23">
         <v>8.76</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>10.85</v>
+      </c>
+      <c r="D23">
+        <v>5.55</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="0"/>
+        <v>39.433962264150942</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6491939622641512</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" si="2"/>
+        <v>23.858447488584474</v>
+      </c>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24">
         <v>8.92</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>10.31</v>
+      </c>
+      <c r="D24">
+        <v>5.54</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="0"/>
+        <v>29.140461215932923</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8659069182389936</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" si="2"/>
+        <v>15.582959641255611</v>
+      </c>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25">
         <v>8.86</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>10.33</v>
+      </c>
+      <c r="D25">
+        <v>5.43</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="0"/>
+        <v>30.000000000000011</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8041853061224487</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="2"/>
+        <v>16.591422121896173</v>
+      </c>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26">
         <v>8.81</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>10.08</v>
+      </c>
+      <c r="D26">
+        <v>5.5</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" si="0"/>
+        <v>27.729257641921389</v>
+      </c>
+      <c r="F26" s="4">
+        <f t="shared" si="1"/>
+        <v>1.9193489082969433</v>
+      </c>
+      <c r="G26" s="4">
+        <f t="shared" si="2"/>
+        <v>14.415437003405215</v>
+      </c>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>10.38</v>
+      </c>
+      <c r="D27">
+        <v>5.49</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="0"/>
+        <v>32.310838445807768</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="1"/>
+        <v>1.7956319018404907</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" si="2"/>
+        <v>17.954545454545453</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28">
         <v>8.74</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>10.18</v>
+      </c>
+      <c r="D28">
+        <v>5.5</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="0"/>
+        <v>30.769230769230759</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8634128205128209</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" si="2"/>
+        <v>16.47597254004576</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29">
         <v>8.65</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="D29">
+        <v>5.51</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="0"/>
+        <v>26.635514018691563</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" si="1"/>
+        <v>2.016581775700935</v>
+      </c>
+      <c r="G29" s="4">
+        <f t="shared" si="2"/>
+        <v>13.179190751445072</v>
+      </c>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30">
         <v>8.89</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>10.26</v>
+      </c>
+      <c r="D30">
+        <v>5.59</v>
+      </c>
+      <c r="E30" s="4">
+        <f t="shared" si="0"/>
+        <v>29.336188436830817</v>
+      </c>
+      <c r="F30" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8994522483940044</v>
+      </c>
+      <c r="G30" s="4">
+        <f t="shared" si="2"/>
+        <v>15.410573678290204</v>
+      </c>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31">
         <v>8.83</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>10.3</v>
+      </c>
+      <c r="D31">
+        <v>5.53</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" si="0"/>
+        <v>30.817610062893092</v>
+      </c>
+      <c r="F31" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8470805031446538</v>
+      </c>
+      <c r="G31" s="4">
+        <f t="shared" si="2"/>
+        <v>16.647791619479055</v>
+      </c>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32">
         <v>8.89</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>10.4</v>
+      </c>
+      <c r="D32">
+        <v>5.58</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" si="0"/>
+        <v>31.327800829875514</v>
+      </c>
+      <c r="F32" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8403406639004152</v>
+      </c>
+      <c r="G32" s="4">
+        <f t="shared" si="2"/>
+        <v>16.985376827896509</v>
+      </c>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33">
         <v>8.06</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>9.42</v>
+      </c>
+      <c r="D33">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" si="0"/>
+        <v>30.909090909090892</v>
+      </c>
+      <c r="F33" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8277881818181818</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" si="2"/>
+        <v>16.873449131513642</v>
+      </c>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34">
         <v>8.86</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>10.54</v>
+      </c>
+      <c r="D34">
+        <v>5.59</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" si="0"/>
+        <v>33.939393939393938</v>
+      </c>
+      <c r="F34" s="4">
+        <f t="shared" si="1"/>
+        <v>1.7859612121212123</v>
+      </c>
+      <c r="G34" s="4">
+        <f t="shared" si="2"/>
+        <v>18.961625282167041</v>
+      </c>
+      <c r="H34" s="4"/>
+      <c r="J34" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35">
         <v>8.86</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>10.57</v>
+      </c>
+      <c r="D35">
+        <v>5.61</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" si="0"/>
+        <v>34.475806451612925</v>
+      </c>
+      <c r="F35" s="4">
+        <f t="shared" si="1"/>
+        <v>1.7823604838709677</v>
+      </c>
+      <c r="G35" s="4">
+        <f t="shared" si="2"/>
+        <v>19.300225733634321</v>
+      </c>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36">
         <v>8.74</v>
       </c>
+      <c r="C36">
+        <v>10.29</v>
+      </c>
+      <c r="D36">
+        <v>5.51</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" si="0"/>
+        <v>32.426778242677806</v>
+      </c>
+      <c r="F36" s="4">
+        <f t="shared" si="1"/>
+        <v>1.8244292887029292</v>
+      </c>
+      <c r="G36" s="4">
+        <f t="shared" si="2"/>
+        <v>17.734553775743695</v>
+      </c>
+      <c r="H36" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A1:H2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>